<commit_message>
New Icons, Localization System. Updated: Project Design Documentation. Unity to 19.4.3f1. Package Updates. Better Conversation System and Camera Controls.
</commit_message>
<xml_diff>
--- a/Project Design/Incurring Costs.xlsx
+++ b/Project Design/Incurring Costs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frozen\Desktop\Project E\Project Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frozen\Desktop\Project F\Project Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A56B8C-17DF-4903-A833-D830EBA4681E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893A290D-249F-4362-A220-FA75B250CD64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E26222B-BBB8-4C44-BEC1-9B00AB8F7830}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -48,18 +48,12 @@
     <t>Astar Pathfinding Project</t>
   </si>
   <si>
-    <t>100.00$</t>
-  </si>
-  <si>
     <t>One-Time Fee</t>
   </si>
   <si>
     <t>PAID</t>
   </si>
   <si>
-    <t>11.99$</t>
-  </si>
-  <si>
     <t xml:space="preserve">LLC Start-up </t>
   </si>
   <si>
@@ -75,18 +69,12 @@
     <t>EIN Number</t>
   </si>
   <si>
-    <t>FREE</t>
-  </si>
-  <si>
     <t>D-U-N-S Number</t>
   </si>
   <si>
     <t>Unity Plus License</t>
   </si>
   <si>
-    <t>399.99$</t>
-  </si>
-  <si>
     <t>Steamworks Game License</t>
   </si>
   <si>
@@ -99,9 +87,6 @@
     <t>Lux URP/LWRP Essentials</t>
   </si>
   <si>
-    <t>20.00$</t>
-  </si>
-  <si>
     <t>UNPAID</t>
   </si>
   <si>
@@ -111,7 +96,22 @@
     <t>Fantastic Fantasy</t>
   </si>
   <si>
-    <t>29.99$</t>
+    <t>Substance Painter</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Unity Asset Store</t>
+  </si>
+  <si>
+    <t>Fmod License</t>
+  </si>
+  <si>
+    <t>I2 Localization</t>
   </si>
 </sst>
 </file>
@@ -119,8 +119,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -177,14 +177,241 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="21">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -195,6 +422,34 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E90C26C5-712B-4BB8-954C-44DF40B3FB51}" name="Table1" displayName="Table1" ref="B2:F8" totalsRowCount="1" headerRowDxfId="20">
+  <autoFilter ref="B2:F7" xr:uid="{9A340518-134D-4415-A466-F96C50A42794}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{5FBAB63D-14FC-41B3-8464-AC63853A50F0}" name="Name" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{99ACC40C-A86D-4880-9E24-266F65E913A0}" name="Price" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{5EC999E3-501A-4E65-86E2-6E2F71C1F591}" name="Type" dataDxfId="17" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0358D402-A08E-4BE1-9062-52946E124039}" name="Status" dataDxfId="16" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{92B9B9DC-4CDA-4A8B-9D5E-C19242EBE080}" name="Date" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{324210E7-FD1D-4F9E-9923-CC24E8C726CA}" name="Table2" displayName="Table2" ref="H2:L12" totalsRowCount="1">
+  <autoFilter ref="H2:L11" xr:uid="{990DA758-9892-4A0D-86ED-C392D18B9A2D}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{791A6FF5-EC57-4050-839F-8BB7BADD28BF}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{512BD180-7EAF-4D53-92AA-C05E98DB8842}" name="Price" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{268265EC-0054-4027-B7FD-8633A0594E6B}" name="Type" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{5E302AB4-E360-49C6-97D6-05E346793921}" name="Status" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5BD63AF5-15C9-49A6-971E-51EC17AD1938}" name="Date" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F83D5BB-C740-4522-AAF0-57A07916D0EE}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,9 +760,12 @@
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,227 +779,320 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8">
+        <v>100</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F3" s="2">
         <v>43979</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="C4" s="8">
+        <v>11.99</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F4" s="2">
         <v>43987</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8">
+        <v>150</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="C5" s="8">
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F5" s="2">
         <v>43997</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="8">
+        <v>300</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="8">
+        <v>29.99</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F6" s="2">
         <v>43998</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
+      <c r="H6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8">
+        <v>45</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>44020</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8">
+        <f>SUBTOTAL(109,Table1[Price])</f>
+        <v>206.98000000000002</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="13">
+        <f>SUBTOTAL(103,Table1[Date])</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="8">
+        <v>100</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="8">
+        <v>20</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="6"/>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="8">
+        <v>244.99</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="6"/>
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="6"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="H12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="I12" s="8">
+        <f>SUBTOTAL(109,Table2[Price])</f>
+        <v>1214.98</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="9">
+        <f>SUBTOTAL(103,Table2[Date])</f>
         <v>9</v>
       </c>
-      <c r="C14" s="7">
-        <v>150</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="7">
-        <v>300</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="E19" s="1"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Game Version 0.1.4. Recipe System and Interface completed. Updated SRP and other NPM Packages. Bugfixes.
</commit_message>
<xml_diff>
--- a/Project Design/Incurring Costs.xlsx
+++ b/Project Design/Incurring Costs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frozen\Desktop\Project F\Project Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893A290D-249F-4362-A220-FA75B250CD64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56056A6F-F9D3-4539-95F3-76EA26D9FF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E26222B-BBB8-4C44-BEC1-9B00AB8F7830}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +114,9 @@
   </si>
   <si>
     <t>I2 Localization</t>
+  </si>
+  <si>
+    <t>Unity Power Tools</t>
   </si>
 </sst>
 </file>
@@ -200,7 +205,11 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -222,7 +231,130 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -248,133 +380,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -425,14 +430,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E90C26C5-712B-4BB8-954C-44DF40B3FB51}" name="Table1" displayName="Table1" ref="B2:F8" totalsRowCount="1" headerRowDxfId="20">
-  <autoFilter ref="B2:F7" xr:uid="{9A340518-134D-4415-A466-F96C50A42794}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E90C26C5-712B-4BB8-954C-44DF40B3FB51}" name="Table1" displayName="Table1" ref="B2:F9" totalsRowCount="1" headerRowDxfId="20">
+  <autoFilter ref="B2:F8" xr:uid="{9A340518-134D-4415-A466-F96C50A42794}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5FBAB63D-14FC-41B3-8464-AC63853A50F0}" name="Name" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{99ACC40C-A86D-4880-9E24-266F65E913A0}" name="Price" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{5EC999E3-501A-4E65-86E2-6E2F71C1F591}" name="Type" dataDxfId="17" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{0358D402-A08E-4BE1-9062-52946E124039}" name="Status" dataDxfId="16" totalsRowDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{92B9B9DC-4CDA-4A8B-9D5E-C19242EBE080}" name="Date" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5FBAB63D-14FC-41B3-8464-AC63853A50F0}" name="Name" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{99ACC40C-A86D-4880-9E24-266F65E913A0}" name="Price" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{5EC999E3-501A-4E65-86E2-6E2F71C1F591}" name="Type" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0358D402-A08E-4BE1-9062-52946E124039}" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{92B9B9DC-4CDA-4A8B-9D5E-C19242EBE080}" name="Date" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -442,11 +447,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{324210E7-FD1D-4F9E-9923-CC24E8C726CA}" name="Table2" displayName="Table2" ref="H2:L12" totalsRowCount="1">
   <autoFilter ref="H2:L11" xr:uid="{990DA758-9892-4A0D-86ED-C392D18B9A2D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{791A6FF5-EC57-4050-839F-8BB7BADD28BF}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{512BD180-7EAF-4D53-92AA-C05E98DB8842}" name="Price" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{268265EC-0054-4027-B7FD-8633A0594E6B}" name="Type" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{5E302AB4-E360-49C6-97D6-05E346793921}" name="Status" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5BD63AF5-15C9-49A6-971E-51EC17AD1938}" name="Date" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{791A6FF5-EC57-4050-839F-8BB7BADD28BF}" name="Name" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{512BD180-7EAF-4D53-92AA-C05E98DB8842}" name="Price" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{268265EC-0054-4027-B7FD-8633A0594E6B}" name="Type" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{5E302AB4-E360-49C6-97D6-05E346793921}" name="Status" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{5BD63AF5-15C9-49A6-971E-51EC17AD1938}" name="Date" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -749,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F83D5BB-C740-4522-AAF0-57A07916D0EE}">
-  <dimension ref="B2:L14"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,17 +964,19 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C8" s="8">
-        <f>SUBTOTAL(109,Table1[Price])</f>
-        <v>206.98000000000002</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="13">
-        <f>SUBTOTAL(103,Table1[Date])</f>
+        <v>29.99</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>44042</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>14</v>
@@ -988,11 +995,19 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="8">
+        <f>SUBTOTAL(109,Table1[Price])</f>
+        <v>236.97000000000003</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="13">
+        <f>SUBTOTAL(103,Table1[Date])</f>
+        <v>6</v>
+      </c>
       <c r="H9" s="12" t="s">
         <v>21</v>
       </c>
@@ -1086,6 +1101,13 @@
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>